<commit_message>
area and min tds sensitivyti analysis done
</commit_message>
<xml_diff>
--- a/Scenarios - provinces.xlsx
+++ b/Scenarios - provinces.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="7180"/>
   </bookViews>
   <sheets>
-    <sheet name="WWR per cluster" sheetId="1" r:id="rId1"/>
+    <sheet name="Baseline" sheetId="1" r:id="rId1"/>
     <sheet name="Priv ag water - Low pop water" sheetId="14" r:id="rId2"/>
     <sheet name="Priv ag water - High pop water" sheetId="15" r:id="rId3"/>
     <sheet name="Sub ag water - Low pop water" sheetId="16" r:id="rId4"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="61">
   <si>
     <t>StartYear</t>
   </si>
@@ -214,18 +214,6 @@
   <si>
     <t>IntensificationRate</t>
   </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
 </sst>
 </file>
 
@@ -233,9 +221,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -307,12 +295,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma [0]" xfId="1" builtinId="6"/>
@@ -634,7 +622,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>